<commit_message>
some more change the logic go routine and wait group, loved the challenges and learning as well, a lot to learn, way to go
</commit_message>
<xml_diff>
--- a/resultAsync.xlsx
+++ b/resultAsync.xlsx
@@ -335,10 +335,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B2" t="str">
-        <v>40320</v>
+        <v>6402373705728000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>